<commit_message>
double weighting issue fixed
</commit_message>
<xml_diff>
--- a/streamlit_wec_full_app_repo/bluechoice_data.xlsx
+++ b/streamlit_wec_full_app_repo/bluechoice_data.xlsx
@@ -3520,10 +3520,15 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Rank</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>WEC Design</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Closeness to Ideal</t>
         </is>
@@ -3539,7 +3544,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.5436710004010832</v>
+        <v>0.6769679823150073</v>
       </c>
     </row>
     <row r="3">
@@ -3548,11 +3553,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Point Absorber</t>
+          <t>Oscillating Water Column</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.4922074191333694</v>
+        <v>0.3505119622780461</v>
       </c>
     </row>
     <row r="4">
@@ -3561,11 +3566,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Oscillating Water Column</t>
+          <t>Point Absorber</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4563289995989168</v>
+        <v>0.2044203284084603</v>
       </c>
     </row>
   </sheetData>
@@ -5979,19 +5984,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2084289779797868</v>
+        <v>0.2211016960397099</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2107868991058177</v>
+        <v>0.2047978497170779</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2105164810687376</v>
+        <v>0.1843855192755456</v>
       </c>
       <c r="E2" t="n">
-        <v>0.175395587587527</v>
+        <v>0.1896748365578238</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1948720542581307</v>
+        <v>0.2000400984098427</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -6004,19 +6009,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2231131126102452</v>
+        <v>0.2343673884268225</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2258193840392323</v>
+        <v>0.2172606660340768</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1848456685710857</v>
+        <v>0.1603201453220851</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2904736781169697</v>
+        <v>0.3110541138651856</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07574815666246695</v>
+        <v>0.07699768635183006</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -6029,19 +6034,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1476229207721817</v>
+        <v>0.1587790613253449</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1858698846550256</v>
+        <v>0.1831033408056535</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2723346548855584</v>
+        <v>0.2418516638648966</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1079095878087588</v>
+        <v>0.1183195610630221</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2862629518784754</v>
+        <v>0.2979463729410828</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>

</xml_diff>